<commit_message>
Sort roads by priority level
</commit_message>
<xml_diff>
--- a/data/roads_parameters_model_paths.xlsx
+++ b/data/roads_parameters_model_paths.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
   <si>
     <t>GDB-Code</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Width</t>
+  </si>
+  <si>
+    <t>Priority level</t>
   </si>
   <si>
     <t>Ausfahrt</t>
@@ -123,7 +126,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,12 +137,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -182,20 +179,20 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -505,7 +502,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -515,7 +512,8 @@
     <col min="2" max="2" style="9" width="17.005" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="10" width="9.005" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="9" width="53.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="17.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -534,20 +532,26 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4"/>
       <c r="E2" s="3">
         <v>6</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
@@ -555,14 +559,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4"/>
       <c r="E3" s="3">
         <v>6</v>
+      </c>
+      <c r="F3" s="1">
+        <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
@@ -570,14 +577,17 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4"/>
       <c r="E4" s="3">
         <v>9</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
@@ -585,14 +595,17 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4"/>
       <c r="E5" s="3">
         <v>6</v>
+      </c>
+      <c r="F5" s="1">
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
@@ -600,13 +613,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="3">
         <v>6</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="3">
+      <c r="F6" s="1">
         <v>6</v>
       </c>
     </row>
@@ -615,14 +631,17 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4"/>
       <c r="E7" s="3">
         <v>6</v>
+      </c>
+      <c r="F7" s="1">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
@@ -630,14 +649,17 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="4"/>
       <c r="E8" s="3">
         <v>4</v>
+      </c>
+      <c r="F8" s="1">
+        <v>8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
@@ -645,31 +667,37 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="6">
         <v>10.2</v>
       </c>
+      <c r="F9" s="1">
+        <v>9</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="46.5">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E10" s="6">
         <v>8</v>
+      </c>
+      <c r="F10" s="1">
+        <v>11</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="46.5">
@@ -677,16 +705,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>6</v>
+        <v>17</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E11" s="6">
         <v>5.21</v>
+      </c>
+      <c r="F11" s="1">
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="73.5">
@@ -694,16 +725,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E12" s="6">
         <v>3.4</v>
+      </c>
+      <c r="F12" s="1">
+        <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
@@ -711,53 +745,65 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="4"/>
       <c r="E13" s="7"/>
+      <c r="F13" s="1">
+        <v>19</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="4"/>
       <c r="E14" s="7"/>
+      <c r="F14" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="4"/>
       <c r="E15" s="7"/>
+      <c r="F15" s="1">
+        <v>21</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="4"/>
       <c r="E16" s="6">
         <v>2.3</v>
+      </c>
+      <c r="F16" s="1">
+        <v>14</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
@@ -765,557 +811,644 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="5"/>
+      <c r="D17" s="4"/>
       <c r="E17" s="6">
         <v>1.2</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="F17" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="4"/>
       <c r="E18" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="F18" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="4"/>
       <c r="E19" s="6">
         <v>2.3</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="F19" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="4"/>
       <c r="E20" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="46.5">
+      <c r="F20" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="44.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>6</v>
+        <v>30</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E21" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+      <c r="F21" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="4"/>
       <c r="E22" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="4"/>
       <c r="E23" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+      <c r="F23" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="4"/>
       <c r="E24" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+      <c r="F24" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="7"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="4"/>
       <c r="E25" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+      <c r="F25" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="7"/>
-      <c r="B26" s="5"/>
+      <c r="B26" s="4"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="5"/>
+      <c r="D26" s="4"/>
       <c r="E26" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+      <c r="F26" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="7"/>
-      <c r="B27" s="5"/>
+      <c r="B27" s="4"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="5"/>
+      <c r="D27" s="4"/>
       <c r="E27" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+      <c r="F27" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="7"/>
-      <c r="B28" s="5"/>
+      <c r="B28" s="4"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="5"/>
+      <c r="D28" s="4"/>
       <c r="E28" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+      <c r="F28" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="7"/>
-      <c r="B29" s="5"/>
+      <c r="B29" s="4"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="5"/>
+      <c r="D29" s="4"/>
       <c r="E29" s="7"/>
+      <c r="F29" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="7"/>
-      <c r="B30" s="5"/>
+      <c r="B30" s="4"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="5"/>
+      <c r="D30" s="4"/>
       <c r="E30" s="7"/>
+      <c r="F30" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="7"/>
-      <c r="B31" s="5"/>
+      <c r="B31" s="4"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="5"/>
+      <c r="D31" s="4"/>
       <c r="E31" s="7"/>
+      <c r="F31" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="7"/>
-      <c r="B32" s="5"/>
+      <c r="B32" s="4"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="5"/>
+      <c r="D32" s="4"/>
       <c r="E32" s="7"/>
+      <c r="F32" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="7"/>
-      <c r="B33" s="5"/>
+      <c r="B33" s="4"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="5"/>
+      <c r="D33" s="4"/>
       <c r="E33" s="7"/>
+      <c r="F33" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="7"/>
-      <c r="B34" s="5"/>
+      <c r="B34" s="4"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="5"/>
+      <c r="D34" s="4"/>
       <c r="E34" s="7"/>
+      <c r="F34" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="7"/>
-      <c r="B35" s="5"/>
+      <c r="B35" s="4"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="5"/>
+      <c r="D35" s="4"/>
       <c r="E35" s="7"/>
+      <c r="F35" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="7"/>
-      <c r="B36" s="5"/>
+      <c r="B36" s="4"/>
       <c r="C36" s="2"/>
-      <c r="D36" s="5"/>
+      <c r="D36" s="4"/>
       <c r="E36" s="7"/>
+      <c r="F36" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="7"/>
-      <c r="B37" s="5"/>
+      <c r="B37" s="4"/>
       <c r="C37" s="2"/>
-      <c r="D37" s="5"/>
+      <c r="D37" s="4"/>
       <c r="E37" s="7"/>
+      <c r="F37" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="7"/>
-      <c r="B38" s="5"/>
+      <c r="B38" s="4"/>
       <c r="C38" s="2"/>
-      <c r="D38" s="5"/>
+      <c r="D38" s="4"/>
       <c r="E38" s="7"/>
+      <c r="F38" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="7"/>
-      <c r="B39" s="5"/>
+      <c r="B39" s="4"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="5"/>
+      <c r="D39" s="4"/>
       <c r="E39" s="7"/>
+      <c r="F39" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="7"/>
-      <c r="B40" s="5"/>
+      <c r="B40" s="4"/>
       <c r="C40" s="2"/>
-      <c r="D40" s="5"/>
+      <c r="D40" s="4"/>
       <c r="E40" s="7"/>
+      <c r="F40" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="7"/>
-      <c r="B41" s="5"/>
+      <c r="B41" s="4"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="5"/>
+      <c r="D41" s="4"/>
       <c r="E41" s="7"/>
+      <c r="F41" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="7"/>
-      <c r="B42" s="5"/>
+      <c r="B42" s="4"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="5"/>
+      <c r="D42" s="4"/>
       <c r="E42" s="7"/>
+      <c r="F42" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="7"/>
-      <c r="B43" s="5"/>
+      <c r="B43" s="4"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="5"/>
+      <c r="D43" s="4"/>
       <c r="E43" s="7"/>
+      <c r="F43" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="7"/>
-      <c r="B44" s="5"/>
+      <c r="B44" s="4"/>
       <c r="C44" s="2"/>
-      <c r="D44" s="5"/>
+      <c r="D44" s="4"/>
       <c r="E44" s="7"/>
+      <c r="F44" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="7"/>
-      <c r="B45" s="5"/>
+      <c r="B45" s="4"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="5"/>
+      <c r="D45" s="4"/>
       <c r="E45" s="7"/>
+      <c r="F45" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="7"/>
-      <c r="B46" s="5"/>
+      <c r="B46" s="4"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="5"/>
+      <c r="D46" s="4"/>
       <c r="E46" s="7"/>
+      <c r="F46" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="7"/>
-      <c r="B47" s="5"/>
+      <c r="B47" s="4"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="5"/>
+      <c r="D47" s="4"/>
       <c r="E47" s="7"/>
+      <c r="F47" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="7"/>
-      <c r="B48" s="5"/>
+      <c r="B48" s="4"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="5"/>
+      <c r="D48" s="4"/>
       <c r="E48" s="7"/>
+      <c r="F48" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
       <c r="A49" s="7"/>
-      <c r="B49" s="5"/>
+      <c r="B49" s="4"/>
       <c r="C49" s="2"/>
-      <c r="D49" s="5"/>
+      <c r="D49" s="4"/>
       <c r="E49" s="7"/>
+      <c r="F49" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="7"/>
-      <c r="B50" s="5"/>
+      <c r="B50" s="4"/>
       <c r="C50" s="2"/>
-      <c r="D50" s="5"/>
+      <c r="D50" s="4"/>
       <c r="E50" s="7"/>
+      <c r="F50" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="7"/>
-      <c r="B51" s="5"/>
+      <c r="B51" s="4"/>
       <c r="C51" s="2"/>
-      <c r="D51" s="5"/>
+      <c r="D51" s="4"/>
       <c r="E51" s="7"/>
+      <c r="F51" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="7"/>
-      <c r="B52" s="5"/>
+      <c r="B52" s="4"/>
       <c r="C52" s="2"/>
-      <c r="D52" s="5"/>
+      <c r="D52" s="4"/>
       <c r="E52" s="7"/>
+      <c r="F52" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="7"/>
-      <c r="B53" s="5"/>
+      <c r="B53" s="4"/>
       <c r="C53" s="2"/>
-      <c r="D53" s="5"/>
+      <c r="D53" s="4"/>
       <c r="E53" s="7"/>
+      <c r="F53" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="7"/>
-      <c r="B54" s="5"/>
+      <c r="B54" s="4"/>
       <c r="C54" s="2"/>
-      <c r="D54" s="5"/>
+      <c r="D54" s="4"/>
       <c r="E54" s="7"/>
+      <c r="F54" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="7"/>
-      <c r="B55" s="5"/>
+      <c r="B55" s="4"/>
       <c r="C55" s="2"/>
-      <c r="D55" s="5"/>
+      <c r="D55" s="4"/>
       <c r="E55" s="7"/>
+      <c r="F55" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="7"/>
-      <c r="B56" s="5"/>
+      <c r="B56" s="4"/>
       <c r="C56" s="2"/>
-      <c r="D56" s="5"/>
+      <c r="D56" s="4"/>
       <c r="E56" s="7"/>
+      <c r="F56" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="7"/>
-      <c r="B57" s="5"/>
+      <c r="B57" s="4"/>
       <c r="C57" s="2"/>
-      <c r="D57" s="5"/>
+      <c r="D57" s="4"/>
       <c r="E57" s="7"/>
+      <c r="F57" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="7"/>
-      <c r="B58" s="5"/>
+      <c r="B58" s="4"/>
       <c r="C58" s="2"/>
-      <c r="D58" s="5"/>
+      <c r="D58" s="4"/>
       <c r="E58" s="7"/>
+      <c r="F58" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="7"/>
-      <c r="B59" s="5"/>
+      <c r="B59" s="4"/>
       <c r="C59" s="2"/>
-      <c r="D59" s="5"/>
+      <c r="D59" s="4"/>
       <c r="E59" s="7"/>
+      <c r="F59" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="7"/>
-      <c r="B60" s="5"/>
+      <c r="B60" s="4"/>
       <c r="C60" s="2"/>
-      <c r="D60" s="5"/>
+      <c r="D60" s="4"/>
       <c r="E60" s="7"/>
+      <c r="F60" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="7"/>
-      <c r="B61" s="5"/>
+      <c r="B61" s="4"/>
       <c r="C61" s="2"/>
-      <c r="D61" s="5"/>
+      <c r="D61" s="4"/>
       <c r="E61" s="7"/>
+      <c r="F61" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="7"/>
-      <c r="B62" s="5"/>
+      <c r="B62" s="4"/>
       <c r="C62" s="2"/>
-      <c r="D62" s="5"/>
+      <c r="D62" s="4"/>
       <c r="E62" s="7"/>
+      <c r="F62" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="7"/>
-      <c r="B63" s="5"/>
+      <c r="B63" s="4"/>
       <c r="C63" s="2"/>
-      <c r="D63" s="5"/>
+      <c r="D63" s="4"/>
       <c r="E63" s="7"/>
+      <c r="F63" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="7"/>
-      <c r="B64" s="5"/>
+      <c r="B64" s="4"/>
       <c r="C64" s="2"/>
-      <c r="D64" s="5"/>
+      <c r="D64" s="4"/>
       <c r="E64" s="7"/>
+      <c r="F64" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="7"/>
-      <c r="B65" s="5"/>
+      <c r="B65" s="4"/>
       <c r="C65" s="2"/>
-      <c r="D65" s="5"/>
+      <c r="D65" s="4"/>
       <c r="E65" s="7"/>
+      <c r="F65" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="7"/>
-      <c r="B66" s="5"/>
+      <c r="B66" s="4"/>
       <c r="C66" s="2"/>
-      <c r="D66" s="5"/>
+      <c r="D66" s="4"/>
       <c r="E66" s="7"/>
+      <c r="F66" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="7"/>
-      <c r="B67" s="5"/>
+      <c r="B67" s="4"/>
       <c r="C67" s="2"/>
-      <c r="D67" s="5"/>
+      <c r="D67" s="4"/>
       <c r="E67" s="7"/>
+      <c r="F67" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="7"/>
-      <c r="B68" s="5"/>
+      <c r="B68" s="4"/>
       <c r="C68" s="2"/>
-      <c r="D68" s="5"/>
+      <c r="D68" s="4"/>
       <c r="E68" s="7"/>
+      <c r="F68" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="7"/>
-      <c r="B69" s="5"/>
+      <c r="B69" s="4"/>
       <c r="C69" s="2"/>
-      <c r="D69" s="5"/>
+      <c r="D69" s="4"/>
       <c r="E69" s="7"/>
+      <c r="F69" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="7"/>
-      <c r="B70" s="5"/>
+      <c r="B70" s="4"/>
       <c r="C70" s="2"/>
-      <c r="D70" s="5"/>
+      <c r="D70" s="4"/>
       <c r="E70" s="7"/>
+      <c r="F70" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="7"/>
-      <c r="B71" s="5"/>
+      <c r="B71" s="4"/>
       <c r="C71" s="2"/>
-      <c r="D71" s="5"/>
+      <c r="D71" s="4"/>
       <c r="E71" s="7"/>
+      <c r="F71" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="7"/>
-      <c r="B72" s="5"/>
+      <c r="B72" s="4"/>
       <c r="C72" s="2"/>
-      <c r="D72" s="5"/>
+      <c r="D72" s="4"/>
       <c r="E72" s="7"/>
+      <c r="F72" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="7"/>
-      <c r="B73" s="5"/>
+      <c r="B73" s="4"/>
       <c r="C73" s="2"/>
-      <c r="D73" s="5"/>
+      <c r="D73" s="4"/>
       <c r="E73" s="7"/>
+      <c r="F73" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="7"/>
-      <c r="B74" s="5"/>
+      <c r="B74" s="4"/>
       <c r="C74" s="2"/>
-      <c r="D74" s="5"/>
+      <c r="D74" s="4"/>
       <c r="E74" s="7"/>
+      <c r="F74" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="7"/>
-      <c r="B75" s="5"/>
+      <c r="B75" s="4"/>
       <c r="C75" s="2"/>
-      <c r="D75" s="5"/>
+      <c r="D75" s="4"/>
       <c r="E75" s="7"/>
+      <c r="F75" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
       <c r="A76" s="7"/>
-      <c r="B76" s="5"/>
+      <c r="B76" s="4"/>
       <c r="C76" s="2"/>
-      <c r="D76" s="5"/>
+      <c r="D76" s="4"/>
       <c r="E76" s="7"/>
+      <c r="F76" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="7"/>
-      <c r="B77" s="5"/>
+      <c r="B77" s="4"/>
       <c r="C77" s="2"/>
-      <c r="D77" s="5"/>
+      <c r="D77" s="4"/>
       <c r="E77" s="7"/>
+      <c r="F77" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
       <c r="A78" s="7"/>
-      <c r="B78" s="5"/>
+      <c r="B78" s="4"/>
       <c r="C78" s="2"/>
-      <c r="D78" s="5"/>
+      <c r="D78" s="4"/>
       <c r="E78" s="7"/>
+      <c r="F78" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
       <c r="A79" s="7"/>
-      <c r="B79" s="5"/>
+      <c r="B79" s="4"/>
       <c r="C79" s="2"/>
-      <c r="D79" s="5"/>
+      <c r="D79" s="4"/>
       <c r="E79" s="7"/>
+      <c r="F79" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="7"/>
-      <c r="B80" s="5"/>
+      <c r="B80" s="4"/>
       <c r="C80" s="2"/>
-      <c r="D80" s="5"/>
+      <c r="D80" s="4"/>
       <c r="E80" s="7"/>
+      <c r="F80" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="7"/>
-      <c r="B81" s="5"/>
+      <c r="B81" s="4"/>
       <c r="C81" s="2"/>
-      <c r="D81" s="5"/>
+      <c r="D81" s="4"/>
       <c r="E81" s="7"/>
+      <c r="F81" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
       <c r="A82" s="7"/>
-      <c r="B82" s="5"/>
+      <c r="B82" s="4"/>
       <c r="C82" s="2"/>
-      <c r="D82" s="5"/>
+      <c r="D82" s="4"/>
       <c r="E82" s="7"/>
+      <c r="F82" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="7"/>
-      <c r="B83" s="5"/>
+      <c r="B83" s="4"/>
       <c r="C83" s="2"/>
-      <c r="D83" s="5"/>
+      <c r="D83" s="4"/>
       <c r="E83" s="7"/>
+      <c r="F83" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
       <c r="A84" s="7"/>
-      <c r="B84" s="5"/>
+      <c r="B84" s="4"/>
       <c r="C84" s="2"/>
-      <c r="D84" s="5"/>
+      <c r="D84" s="4"/>
       <c r="E84" s="7"/>
+      <c r="F84" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
       <c r="A85" s="7"/>
-      <c r="B85" s="5"/>
+      <c r="B85" s="4"/>
       <c r="C85" s="2"/>
-      <c r="D85" s="5"/>
+      <c r="D85" s="4"/>
       <c r="E85" s="7"/>
+      <c r="F85" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="7"/>
-      <c r="B86" s="5"/>
+      <c r="B86" s="4"/>
       <c r="C86" s="2"/>
-      <c r="D86" s="5"/>
+      <c r="D86" s="4"/>
       <c r="E86" s="7"/>
+      <c r="F86" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
       <c r="A87" s="7"/>
-      <c r="B87" s="5"/>
+      <c r="B87" s="4"/>
       <c r="C87" s="2"/>
-      <c r="D87" s="5"/>
+      <c r="D87" s="4"/>
       <c r="E87" s="7"/>
+      <c r="F87" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>